<commit_message>
Update regression output formatting and model comparisons
</commit_message>
<xml_diff>
--- a/outputs/regression_outs_no_retal_v2.xlsx
+++ b/outputs/regression_outs_no_retal_v2.xlsx
@@ -1,239 +1,232 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elisabethsilver/Documents/EEOC-AWD/outputs/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A6B4CC-1FB1-6D46-97EA-732AB78F44C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView xWindow="14280" yWindow="1800" windowWidth="15700" windowHeight="8820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="69">
-  <si>
-    <t>Predictor</t>
-  </si>
-  <si>
-    <t>Predictor_pretty</t>
-  </si>
-  <si>
-    <t>model1_b</t>
-  </si>
-  <si>
-    <t>model1_se_b</t>
-  </si>
-  <si>
-    <t>model2_b</t>
-  </si>
-  <si>
-    <t>model2_se_b</t>
-  </si>
-  <si>
-    <t>model3_b</t>
-  </si>
-  <si>
-    <t>model3_se_b</t>
-  </si>
-  <si>
-    <t>model4_b</t>
-  </si>
-  <si>
-    <t>model4_se_b</t>
-  </si>
-  <si>
-    <t>(Intercept)</t>
-  </si>
-  <si>
-    <t>Intercept</t>
-  </si>
-  <si>
-    <t>2.84***</t>
-  </si>
-  <si>
-    <t>0.79</t>
-  </si>
-  <si>
-    <t>3.43***</t>
-  </si>
-  <si>
-    <t>0.80</t>
-  </si>
-  <si>
-    <t>2.93***</t>
-  </si>
-  <si>
-    <t>4.59***</t>
-  </si>
-  <si>
-    <t>0.99</t>
-  </si>
-  <si>
-    <t>acs_nonwhite_prop</t>
-  </si>
-  <si>
-    <t>POC representation</t>
-  </si>
-  <si>
-    <t>0.07***</t>
-  </si>
-  <si>
-    <t>0.00</t>
-  </si>
-  <si>
-    <t>0.05***</t>
-  </si>
-  <si>
-    <t>0.01</t>
-  </si>
-  <si>
-    <t>0.06***</t>
-  </si>
-  <si>
-    <t>0.04**</t>
-  </si>
-  <si>
-    <t>mrp_ideology</t>
-  </si>
-  <si>
-    <t>Conservatism</t>
-  </si>
-  <si>
-    <t>1.53*</t>
-  </si>
-  <si>
-    <t>0.67</t>
-  </si>
-  <si>
-    <t>-1.34</t>
-  </si>
-  <si>
-    <t>0.93</t>
-  </si>
-  <si>
-    <t>1.56*</t>
-  </si>
-  <si>
-    <t>-4.13</t>
-  </si>
-  <si>
-    <t>2.20</t>
-  </si>
-  <si>
-    <t>acs_unemploy_white</t>
-  </si>
-  <si>
-    <t>White unemployment</t>
-  </si>
-  <si>
-    <t>0.02</t>
-  </si>
-  <si>
-    <t>0.04</t>
-  </si>
-  <si>
-    <t>-0.13</t>
-  </si>
-  <si>
-    <t>0.08</t>
-  </si>
-  <si>
-    <t>log_total_pop</t>
-  </si>
-  <si>
-    <t>Total population (log-transformed)</t>
-  </si>
-  <si>
-    <t>-0.20**</t>
-  </si>
-  <si>
-    <t>0.07</t>
-  </si>
-  <si>
-    <t>-0.19**</t>
-  </si>
-  <si>
-    <t>-0.21**</t>
-  </si>
-  <si>
-    <t>acs_nonwhite_prop:mrp_ideology</t>
-  </si>
-  <si>
-    <t>POC representation x Conservatism</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>0.10***</t>
-  </si>
-  <si>
-    <t>0.05</t>
-  </si>
-  <si>
-    <t>acs_nonwhite_prop:acs_unemploy_white</t>
-  </si>
-  <si>
-    <t>POC representation x White unemployment</t>
-  </si>
-  <si>
-    <t>mrp_ideology:acs_unemploy_white</t>
-  </si>
-  <si>
-    <t>Conservatism x White unemployment</t>
-  </si>
-  <si>
-    <t>0.39</t>
-  </si>
-  <si>
-    <t>0.30</t>
-  </si>
-  <si>
-    <t>acs_nonwhite_prop:mrp_ideology:acs_unemploy_white</t>
-  </si>
-  <si>
-    <t>POC representation x Conservatism x White unemployment</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>0.079</t>
-  </si>
-  <si>
-    <t>0.085</t>
-  </si>
-  <si>
-    <t>0.087</t>
-  </si>
-  <si>
-    <t>Change in R2</t>
-  </si>
-  <si>
-    <t>19.66***</t>
-  </si>
-  <si>
-    <t>0.57</t>
-  </si>
-  <si>
-    <t>3.60*</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+  <si>
+    <t xml:space="preserve">Predictor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Predictor_pretty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model1_b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model1_se_b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model2_b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model2_se_b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model3_b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model3_se_b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model2a_b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model2a_se_b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Intercept)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intercept</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.84***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.79</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.43***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.59***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.93***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">acs_nonwhite_prop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POC representation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.07***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.05***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.04**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.06***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mrp_ideology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conservatism</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.53*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.67</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.93</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-4.13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.56*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">acs_unemploy_white</t>
+  </si>
+  <si>
+    <t xml:space="preserve">White unemployment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">log_total_pop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total population (log-transformed)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.20**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.21**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.19**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">acs_nonwhite_prop:mrp_ideology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POC representation x Conservatism</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.10***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">acs_nonwhite_prop:acs_unemploy_white</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POC representation x White unemployment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mrp_ideology:acs_unemploy_white</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conservatism x White unemployment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">acs_nonwhite_prop:mrp_ideology:acs_unemploy_white</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POC representation x Conservatism x White unemployment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.079</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.085</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.087</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change in R2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19.66***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.60*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.57</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -269,15 +262,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -559,16 +543,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
-    </sheetView>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -600,7 +582,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -623,16 +605,16 @@
         <v>16</v>
       </c>
       <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
         <v>15</v>
       </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -664,7 +646,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -687,16 +669,16 @@
         <v>33</v>
       </c>
       <c r="H4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" t="s">
         <v>30</v>
       </c>
-      <c r="I4" t="s">
-        <v>34</v>
-      </c>
-      <c r="J4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -716,19 +698,19 @@
         <v>38</v>
       </c>
       <c r="G5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" t="s">
         <v>22</v>
-      </c>
-      <c r="H5" t="s">
-        <v>39</v>
-      </c>
-      <c r="I5" t="s">
-        <v>40</v>
       </c>
       <c r="J5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -760,7 +742,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7">
       <c r="A7" t="s">
         <v>48</v>
       </c>
@@ -780,19 +762,19 @@
         <v>38</v>
       </c>
       <c r="G7" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="H7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="I7" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="J7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -824,7 +806,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -844,19 +826,19 @@
         <v>50</v>
       </c>
       <c r="G9" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="H9" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="I9" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="J9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10">
       <c r="A10" t="s">
         <v>59</v>
       </c>
@@ -876,19 +858,19 @@
         <v>50</v>
       </c>
       <c r="G10" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="H10" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="I10" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="J10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11">
       <c r="A11" t="s">
         <v>61</v>
       </c>
@@ -911,16 +893,16 @@
         <v>50</v>
       </c>
       <c r="H11" t="s">
+        <v>64</v>
+      </c>
+      <c r="I11" t="s">
+        <v>50</v>
+      </c>
+      <c r="J11" t="s">
         <v>62</v>
       </c>
-      <c r="I11" t="s">
-        <v>50</v>
-      </c>
-      <c r="J11" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12">
       <c r="A12" t="s">
         <v>65</v>
       </c>
@@ -954,6 +936,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>